<commit_message>
some minor fixes / enhancements
</commit_message>
<xml_diff>
--- a/short_test.xlsx
+++ b/short_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vi_ah\OneDrive - TUNI.fi\Opiskelut\D-työ\matlab\EEG_validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vi_ah\OneDrive - TUNI.fi\Opiskelut\D-työ\matlab\EEG_validator_git\eeg-validator-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -71,10 +71,10 @@
     <t>2020_G1xx</t>
   </si>
   <si>
-    <t>xxxeeecx</t>
-  </si>
-  <si>
     <t>2017_G1</t>
+  </si>
+  <si>
+    <t>eeeeeexc</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +501,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -519,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>7</v>
@@ -828,6 +828,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizId xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <TeamsChannelId xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Invited_Members xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <AppVersion xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Templates xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <NotebookType xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <FolderType xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <MigrationWizIdSecurityGroups xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Has_Leaders_Only_SectionGroup xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Owner xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <MigrationWizIdPermissions xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <MigrationWizIdDocumentLibraryPermissions xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Invited_Leaders xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <MigrationWizIdPermissionLevels xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Members xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Member_Groups xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <CultureName xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
+    <Leaders xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100AE97E8C6A1A56B4087C1BCCE3C4DD0BE" ma:contentTypeVersion="35" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="7f9f0248149a3b48a910e799add6d3e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5281d71e-083a-4851-b000-6f17641b21c3" xmlns:ns4="b5920e61-5a32-4c5a-bdfa-bf4c57638ce0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e172c03af79af8044cdbd18208dae289" ns3:_="" ns4:_="">
     <xsd:import namespace="5281d71e-083a-4851-b000-6f17641b21c3"/>
@@ -1246,83 +1308,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizId xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <TeamsChannelId xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Invited_Members xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <AppVersion xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Templates xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <NotebookType xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <FolderType xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <MigrationWizIdSecurityGroups xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Has_Leaders_Only_SectionGroup xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Owner xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <MigrationWizIdPermissions xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <MigrationWizIdDocumentLibraryPermissions xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Invited_Leaders xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <MigrationWizIdPermissionLevels xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Members xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Member_Groups xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <CultureName xmlns="5281d71e-083a-4851-b000-6f17641b21c3" xsi:nil="true"/>
-    <Leaders xmlns="5281d71e-083a-4851-b000-6f17641b21c3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BCB873-451F-4A7D-9C90-271A8B748275}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41FC4E6E-30DC-4577-805A-6CFFA96232C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5281d71e-083a-4851-b000-6f17641b21c3"/>
-    <ds:schemaRef ds:uri="b5920e61-5a32-4c5a-bdfa-bf4c57638ce0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1345,9 +1334,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41FC4E6E-30DC-4577-805A-6CFFA96232C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BCB873-451F-4A7D-9C90-271A8B748275}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5281d71e-083a-4851-b000-6f17641b21c3"/>
+    <ds:schemaRef ds:uri="b5920e61-5a32-4c5a-bdfa-bf4c57638ce0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>